<commit_message>
added the results of DESeq2
</commit_message>
<xml_diff>
--- a/Muscle_gene_summary_includeMF.xlsx
+++ b/Muscle_gene_summary_includeMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Documents/Bioinformatics/MetaAnalysisProject_Apr2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E675B57-B3B4-5445-B4C7-306D5E5B6860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B3583C-BF1D-A94A-B693-B039DD0BBEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1660" windowWidth="27200" windowHeight="13000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1660" windowWidth="27200" windowHeight="13000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acute" sheetId="11" r:id="rId1"/>
@@ -1692,12 +1692,12 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7803,9 +7803,9 @@
   </sheetPr>
   <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F11" sqref="F11"/>
+      <selection pane="topRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -8732,7 +8732,7 @@
       </c>
     </row>
     <row r="10" spans="1:39" s="95" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="139" t="s">
+      <c r="A10" s="141" t="s">
         <v>206</v>
       </c>
       <c r="B10" s="92" t="s">
@@ -8812,7 +8812,7 @@
       </c>
     </row>
     <row r="11" spans="1:39" s="95" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="139" t="s">
+      <c r="A11" s="141" t="s">
         <v>206</v>
       </c>
       <c r="B11" s="92" t="s">
@@ -9045,8 +9045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E983AE-3E94-4A77-A645-69889912A19D}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -9276,7 +9276,7 @@
       <c r="Y3" s="110"/>
     </row>
     <row r="4" spans="1:25" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="141" t="s">
+      <c r="A4" s="140" t="s">
         <v>278</v>
       </c>
       <c r="B4" s="110" t="s">
@@ -9346,7 +9346,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="141" t="s">
+      <c r="A5" s="140" t="s">
         <v>206</v>
       </c>
       <c r="B5" s="110" t="s">
@@ -9475,7 +9475,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="140" t="s">
+      <c r="A7" s="139" t="s">
         <v>292</v>
       </c>
       <c r="B7" s="110" t="s">

</xml_diff>

<commit_message>
added memos to GSE162730 (aging): no young samples?
</commit_message>
<xml_diff>
--- a/Muscle_gene_summary_includeMF.xlsx
+++ b/Muscle_gene_summary_includeMF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Documents/Bioinformatics/MetaAnalysisProject_Apr2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B3583C-BF1D-A94A-B693-B039DD0BBEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA72BF87-6C03-D846-A4C2-CFD1D4516DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1660" windowWidth="27200" windowHeight="13000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1660" windowWidth="27200" windowHeight="13000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acute" sheetId="11" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="307">
   <si>
     <t>Age</t>
   </si>
@@ -988,6 +988,9 @@
   </si>
   <si>
     <t>https://pubmed.ncbi.nlm.nih.gov/33705535/</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/33705535/</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1021,6 +1024,9 @@
   <si>
     <t>-</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>no young samples? miRna-seq / Ribo-seq</t>
   </si>
 </sst>
 </file>
@@ -7803,9 +7809,9 @@
   </sheetPr>
   <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D11" sqref="D11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -7961,7 +7967,7 @@
     </row>
     <row r="2" spans="1:39" s="95" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="104" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B2" s="113" t="s">
         <v>145</v>
@@ -7971,22 +7977,22 @@
       </c>
       <c r="D2" s="113"/>
       <c r="E2" s="130" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F2" s="105" t="s">
         <v>143</v>
       </c>
       <c r="G2" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="H2" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="I2" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="J2" s="105" t="s">
         <v>304</v>
-      </c>
-      <c r="H2" s="130" t="s">
-        <v>304</v>
-      </c>
-      <c r="I2" s="105" t="s">
-        <v>302</v>
-      </c>
-      <c r="J2" s="105" t="s">
-        <v>303</v>
       </c>
       <c r="K2" s="106" t="s">
         <v>5</v>
@@ -8069,22 +8075,22 @@
       </c>
       <c r="D3" s="113"/>
       <c r="E3" s="130" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F3" s="105" t="s">
         <v>143</v>
       </c>
       <c r="G3" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="H3" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="I3" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="J3" s="105" t="s">
         <v>304</v>
-      </c>
-      <c r="H3" s="130" t="s">
-        <v>304</v>
-      </c>
-      <c r="I3" s="105" t="s">
-        <v>302</v>
-      </c>
-      <c r="J3" s="105" t="s">
-        <v>303</v>
       </c>
       <c r="K3" s="106" t="s">
         <v>5</v>
@@ -8167,22 +8173,22 @@
       </c>
       <c r="D4" s="113"/>
       <c r="E4" s="130" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F4" s="105" t="s">
         <v>143</v>
       </c>
       <c r="G4" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="H4" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="I4" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="J4" s="105" t="s">
         <v>304</v>
-      </c>
-      <c r="H4" s="130" t="s">
-        <v>304</v>
-      </c>
-      <c r="I4" s="105" t="s">
-        <v>302</v>
-      </c>
-      <c r="J4" s="105" t="s">
-        <v>303</v>
       </c>
       <c r="K4" s="106" t="s">
         <v>5</v>
@@ -8265,22 +8271,22 @@
       </c>
       <c r="D5" s="113"/>
       <c r="E5" s="130" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F5" s="105" t="s">
         <v>143</v>
       </c>
       <c r="G5" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="H5" s="130" t="s">
+        <v>305</v>
+      </c>
+      <c r="I5" s="105" t="s">
+        <v>303</v>
+      </c>
+      <c r="J5" s="105" t="s">
         <v>304</v>
-      </c>
-      <c r="H5" s="130" t="s">
-        <v>304</v>
-      </c>
-      <c r="I5" s="105" t="s">
-        <v>302</v>
-      </c>
-      <c r="J5" s="105" t="s">
-        <v>303</v>
       </c>
       <c r="K5" s="106" t="s">
         <v>5</v>
@@ -8756,7 +8762,7 @@
         <v>291</v>
       </c>
       <c r="J10" s="129" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K10" s="95" t="s">
         <v>10</v>
@@ -8913,10 +8919,10 @@
       <c r="G12" s="134"/>
       <c r="H12" s="134"/>
       <c r="I12" s="108" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="J12" s="108" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K12" s="106" t="s">
         <v>5</v>
@@ -8983,10 +8989,10 @@
       <c r="G13" s="134"/>
       <c r="H13" s="134"/>
       <c r="I13" s="108" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="J13" s="108" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K13" s="106" t="s">
         <v>5</v>
@@ -9045,8 +9051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E983AE-3E94-4A77-A645-69889912A19D}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -9166,7 +9172,7 @@
         <v>290</v>
       </c>
       <c r="J2" s="105" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K2" s="110" t="s">
         <v>199</v>
@@ -9232,7 +9238,7 @@
         <v>290</v>
       </c>
       <c r="J3" s="105" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="K3" s="110" t="s">
         <v>199</v>
@@ -9286,7 +9292,7 @@
         <v>277</v>
       </c>
       <c r="D4" s="105" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="E4" s="105" t="s">
         <v>283</v>
@@ -9300,7 +9306,7 @@
         <v>291</v>
       </c>
       <c r="J4" s="105" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K4" s="110" t="s">
         <v>221</v>
@@ -9356,7 +9362,7 @@
         <v>277</v>
       </c>
       <c r="D5" s="105" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="E5" s="105" t="s">
         <v>283</v>
@@ -9370,7 +9376,7 @@
         <v>291</v>
       </c>
       <c r="J5" s="105" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="K5" s="110" t="s">
         <v>221</v>
@@ -9438,7 +9444,7 @@
         <v>289</v>
       </c>
       <c r="J6" s="91" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K6" s="110" t="s">
         <v>229</v>

</xml_diff>

<commit_message>
added a memo to GSE162730 (aging): no young samples?
</commit_message>
<xml_diff>
--- a/Muscle_gene_summary_includeMF.xlsx
+++ b/Muscle_gene_summary_includeMF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Documents/Bioinformatics/MetaAnalysisProject_Apr2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA72BF87-6C03-D846-A4C2-CFD1D4516DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2DB221-E870-E942-97D4-733EE9778568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1660" windowWidth="27200" windowHeight="13000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1316,7 +1316,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1664,7 +1664,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1704,6 +1703,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7820,9 +7825,9 @@
     <col min="2" max="2" width="9.83203125" style="111"/>
     <col min="3" max="3" width="11.33203125" style="111" customWidth="1"/>
     <col min="4" max="4" width="28" style="111" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="138" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="137" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" style="99" customWidth="1"/>
-    <col min="7" max="8" width="17" style="135" customWidth="1"/>
+    <col min="7" max="8" width="17" style="134" customWidth="1"/>
     <col min="9" max="9" width="69" style="99" customWidth="1"/>
     <col min="10" max="10" width="62.5" style="99" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" style="99" bestFit="1" customWidth="1"/>
@@ -7859,16 +7864,16 @@
       <c r="D1" s="117" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="136" t="s">
+      <c r="E1" s="135" t="s">
         <v>282</v>
       </c>
       <c r="F1" s="118" t="s">
         <v>267</v>
       </c>
-      <c r="G1" s="131" t="s">
+      <c r="G1" s="130" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="131" t="s">
+      <c r="H1" s="130" t="s">
         <v>286</v>
       </c>
       <c r="I1" s="118" t="s">
@@ -7886,22 +7891,22 @@
       <c r="M1" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="127" t="s">
+      <c r="N1" s="126" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="128" t="s">
+      <c r="O1" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="128" t="s">
+      <c r="P1" s="127" t="s">
         <v>122</v>
       </c>
       <c r="Q1" s="118" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="128" t="s">
+      <c r="R1" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="128" t="s">
+      <c r="S1" s="127" t="s">
         <v>73</v>
       </c>
       <c r="T1" s="118" t="s">
@@ -7928,19 +7933,19 @@
       <c r="AA1" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="127" t="s">
+      <c r="AB1" s="126" t="s">
         <v>121</v>
       </c>
-      <c r="AC1" s="127" t="s">
+      <c r="AC1" s="126" t="s">
         <v>125</v>
       </c>
-      <c r="AD1" s="127" t="s">
+      <c r="AD1" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="AE1" s="128" t="s">
+      <c r="AE1" s="127" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="128" t="s">
+      <c r="AF1" s="127" t="s">
         <v>169</v>
       </c>
       <c r="AG1" s="118" t="s">
@@ -7972,20 +7977,20 @@
       <c r="B2" s="113" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="126" t="s">
+      <c r="C2" s="125" t="s">
         <v>269</v>
       </c>
       <c r="D2" s="113"/>
-      <c r="E2" s="130" t="s">
+      <c r="E2" s="129" t="s">
         <v>305</v>
       </c>
       <c r="F2" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="130" t="s">
+      <c r="G2" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="H2" s="130" t="s">
+      <c r="H2" s="129" t="s">
         <v>305</v>
       </c>
       <c r="I2" s="105" t="s">
@@ -8070,20 +8075,20 @@
       <c r="B3" s="113" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="126" t="s">
+      <c r="C3" s="125" t="s">
         <v>269</v>
       </c>
       <c r="D3" s="113"/>
-      <c r="E3" s="130" t="s">
+      <c r="E3" s="129" t="s">
         <v>305</v>
       </c>
       <c r="F3" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="G3" s="130" t="s">
+      <c r="G3" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="H3" s="130" t="s">
+      <c r="H3" s="129" t="s">
         <v>305</v>
       </c>
       <c r="I3" s="105" t="s">
@@ -8168,20 +8173,20 @@
       <c r="B4" s="113" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="126" t="s">
+      <c r="C4" s="125" t="s">
         <v>269</v>
       </c>
       <c r="D4" s="113"/>
-      <c r="E4" s="130" t="s">
+      <c r="E4" s="129" t="s">
         <v>305</v>
       </c>
       <c r="F4" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="130" t="s">
+      <c r="G4" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="H4" s="130" t="s">
+      <c r="H4" s="129" t="s">
         <v>305</v>
       </c>
       <c r="I4" s="105" t="s">
@@ -8266,20 +8271,20 @@
       <c r="B5" s="113" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="126" t="s">
+      <c r="C5" s="125" t="s">
         <v>269</v>
       </c>
       <c r="D5" s="113"/>
-      <c r="E5" s="130" t="s">
+      <c r="E5" s="129" t="s">
         <v>305</v>
       </c>
       <c r="F5" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="130" t="s">
+      <c r="G5" s="129" t="s">
         <v>305</v>
       </c>
-      <c r="H5" s="130" t="s">
+      <c r="H5" s="129" t="s">
         <v>305</v>
       </c>
       <c r="I5" s="105" t="s">
@@ -8368,14 +8373,14 @@
         <v>273</v>
       </c>
       <c r="D6" s="113"/>
-      <c r="E6" s="137" t="s">
+      <c r="E6" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F6" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="132"/>
-      <c r="H6" s="132"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
       <c r="I6" s="105" t="s">
         <v>293</v>
       </c>
@@ -8463,14 +8468,14 @@
         <v>273</v>
       </c>
       <c r="D7" s="113"/>
-      <c r="E7" s="137" t="s">
+      <c r="E7" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F7" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="131"/>
       <c r="I7" s="105" t="s">
         <v>293</v>
       </c>
@@ -8558,14 +8563,14 @@
         <v>273</v>
       </c>
       <c r="D8" s="113"/>
-      <c r="E8" s="137" t="s">
+      <c r="E8" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F8" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131"/>
       <c r="I8" s="105" t="s">
         <v>293</v>
       </c>
@@ -8653,14 +8658,14 @@
         <v>273</v>
       </c>
       <c r="D9" s="113"/>
-      <c r="E9" s="137" t="s">
+      <c r="E9" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F9" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="G9" s="132"/>
-      <c r="H9" s="132"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="131"/>
       <c r="I9" s="105" t="s">
         <v>293</v>
       </c>
@@ -8738,7 +8743,7 @@
       </c>
     </row>
     <row r="10" spans="1:39" s="95" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="141" t="s">
+      <c r="A10" s="140" t="s">
         <v>206</v>
       </c>
       <c r="B10" s="92" t="s">
@@ -8750,18 +8755,18 @@
       <c r="D10" s="105" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="137" t="s">
+      <c r="E10" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F10" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="G10" s="133"/>
-      <c r="H10" s="133"/>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
       <c r="I10" s="95" t="s">
         <v>291</v>
       </c>
-      <c r="J10" s="129" t="s">
+      <c r="J10" s="128" t="s">
         <v>297</v>
       </c>
       <c r="K10" s="95" t="s">
@@ -8818,7 +8823,7 @@
       </c>
     </row>
     <row r="11" spans="1:39" s="95" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="141" t="s">
+      <c r="A11" s="140" t="s">
         <v>206</v>
       </c>
       <c r="B11" s="92" t="s">
@@ -8830,18 +8835,18 @@
       <c r="D11" s="105" t="s">
         <v>281</v>
       </c>
-      <c r="E11" s="137" t="s">
+      <c r="E11" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F11" s="95" t="s">
         <v>223</v>
       </c>
-      <c r="G11" s="133"/>
-      <c r="H11" s="133"/>
+      <c r="G11" s="132"/>
+      <c r="H11" s="132"/>
       <c r="I11" s="95" t="s">
         <v>291</v>
       </c>
-      <c r="J11" s="129" t="s">
+      <c r="J11" s="128" t="s">
         <v>296</v>
       </c>
       <c r="K11" s="95" t="s">
@@ -8910,14 +8915,14 @@
       <c r="D12" s="115" t="s">
         <v>275</v>
       </c>
-      <c r="E12" s="137" t="s">
+      <c r="E12" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F12" s="108" t="s">
         <v>141</v>
       </c>
-      <c r="G12" s="134"/>
-      <c r="H12" s="134"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="133"/>
       <c r="I12" s="108" t="s">
         <v>300</v>
       </c>
@@ -8980,14 +8985,14 @@
       <c r="D13" s="115" t="s">
         <v>275</v>
       </c>
-      <c r="E13" s="137" t="s">
+      <c r="E13" s="136" t="s">
         <v>283</v>
       </c>
       <c r="F13" s="108" t="s">
         <v>141</v>
       </c>
-      <c r="G13" s="134"/>
-      <c r="H13" s="134"/>
+      <c r="G13" s="133"/>
+      <c r="H13" s="133"/>
       <c r="I13" s="108" t="s">
         <v>300</v>
       </c>
@@ -9052,7 +9057,7 @@
   <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -9153,14 +9158,14 @@
       <c r="A2" s="110" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="141" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="125" t="s">
+      <c r="C2" s="142" t="s">
         <v>277</v>
       </c>
       <c r="D2" s="105"/>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="141" t="s">
         <v>283</v>
       </c>
       <c r="F2" s="110" t="s">
@@ -9219,14 +9224,14 @@
       <c r="A3" s="110" t="s">
         <v>198</v>
       </c>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="141" t="s">
         <v>276</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="142" t="s">
         <v>277</v>
       </c>
       <c r="D3" s="105"/>
-      <c r="E3" s="105" t="s">
+      <c r="E3" s="141" t="s">
         <v>283</v>
       </c>
       <c r="F3" s="110" t="s">
@@ -9282,19 +9287,19 @@
       <c r="Y3" s="110"/>
     </row>
     <row r="4" spans="1:25" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="139" t="s">
         <v>278</v>
       </c>
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="141" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="142" t="s">
         <v>277</v>
       </c>
       <c r="D4" s="105" t="s">
         <v>306</v>
       </c>
-      <c r="E4" s="105" t="s">
+      <c r="E4" s="141" t="s">
         <v>283</v>
       </c>
       <c r="F4" s="91" t="s">
@@ -9352,19 +9357,19 @@
       </c>
     </row>
     <row r="5" spans="1:25" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="140" t="s">
+      <c r="A5" s="139" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="141" t="s">
         <v>276</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="142" t="s">
         <v>277</v>
       </c>
       <c r="D5" s="105" t="s">
         <v>306</v>
       </c>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="141" t="s">
         <v>283</v>
       </c>
       <c r="F5" s="91" t="s">
@@ -9425,14 +9430,14 @@
       <c r="A6" s="91" t="s">
         <v>279</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="141" t="s">
         <v>276</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="141" t="s">
         <v>277</v>
       </c>
       <c r="D6" s="105"/>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="141" t="s">
         <v>283</v>
       </c>
       <c r="F6" s="97" t="s">
@@ -9481,17 +9486,17 @@
       </c>
     </row>
     <row r="7" spans="1:25" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="138" t="s">
         <v>292</v>
       </c>
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="141" t="s">
         <v>276</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="142" t="s">
         <v>277</v>
       </c>
       <c r="D7" s="105"/>
-      <c r="E7" s="105" t="s">
+      <c r="E7" s="141" t="s">
         <v>283</v>
       </c>
       <c r="F7" s="91" t="s">

</xml_diff>